<commit_message>
Ultima Versão EAP - Guilherme Lista de Evento atualizada - Guilherme
</commit_message>
<xml_diff>
--- a/TCC - Monografia/Modelo de Análise dos Eventos.xlsx
+++ b/TCC - Monografia/Modelo de Análise dos Eventos.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Desktop\pos-fit-es10\trunk\TCC - Monografia\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4170" activeTab="2"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>Capacidades</t>
   </si>
@@ -102,13 +97,25 @@
   </si>
   <si>
     <t>Gerente paga as contas que estão vencendo</t>
+  </si>
+  <si>
+    <t>Registrar Motoboy</t>
+  </si>
+  <si>
+    <t>Registrar Veículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motoboy envia informações sobre seus dados pessoais. </t>
+  </si>
+  <si>
+    <t>Proprietário envia informações sobre o novo veículo para o Coordenador Administrativo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,10 +430,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -446,67 +453,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1381125" y="3086100"/>
-          <a:ext cx="10125075" cy="2524125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -563,7 +510,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -595,10 +542,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,7 +576,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -806,14 +751,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
@@ -822,7 +767,7 @@
     <col min="5" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="18.75" customHeight="1">
       <c r="E1" s="19" t="s">
         <v>9</v>
       </c>
@@ -833,7 +778,7 @@
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="35.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -863,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="33.75" customHeight="1">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -885,7 +830,7 @@
       <c r="I3" s="10"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="21"/>
       <c r="B4" s="27"/>
       <c r="C4" s="1">
@@ -903,7 +848,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="45">
       <c r="A5" s="22"/>
       <c r="B5" s="28"/>
       <c r="C5" s="1">
@@ -921,7 +866,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="34.5" customHeight="1">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -943,7 +888,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="34.5" customHeight="1">
       <c r="A7" s="24"/>
       <c r="B7" s="30"/>
       <c r="C7" s="1">
@@ -961,7 +906,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="32.25" customHeight="1">
       <c r="A8" s="25"/>
       <c r="B8" s="31"/>
       <c r="C8" s="1">
@@ -979,7 +924,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="72" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
@@ -1001,7 +946,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="72" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
@@ -1038,14 +983,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1053,14 +998,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
@@ -1069,7 +1014,7 @@
     <col min="5" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="18.75" customHeight="1">
       <c r="E1" s="19" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1025,7 @@
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="35.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="72" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
@@ -1132,7 +1077,7 @@
       <c r="I3" s="10"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="72" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1085,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>19</v>
@@ -1153,6 +1098,50 @@
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" ht="84.75" customHeight="1">
+      <c r="A5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="67.5" customHeight="1">
+      <c r="A6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="13">
+        <v>4</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1160,6 +1149,5 @@
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>